<commit_message>
Update comments on parameter input for this project. Echo parameters to output file. Eliminate spaces in site names.
Signed-off-by: Lira, Carl <lira@msu.edu>
</commit_message>
<xml_diff>
--- a/Input/GAMMAPA/Input Template Main.xlsx
+++ b/Input/GAMMAPA/Input Template Main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lira.EGR\Documents\repos\MDNAproject\Input\GAMMAPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D178E658-0061-449D-81AC-75A43AFD18D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13625C61-0FF5-414C-B667-98531B2A1C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,18 +68,12 @@
     <t>source</t>
   </si>
   <si>
-    <t>hydroxyl O</t>
-  </si>
-  <si>
     <t>METHANOL</t>
   </si>
   <si>
     <t>noccur</t>
   </si>
   <si>
-    <t>hydroxyl H</t>
-  </si>
-  <si>
     <t>host1</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>n bonding pairs</t>
+  </si>
+  <si>
+    <t>hydroxyl_O_MeOH</t>
+  </si>
+  <si>
+    <t>hydroxyl_H_MeOH</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,16 +529,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -553,28 +553,28 @@
         <v>9</v>
       </c>
       <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>29</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>30</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>32</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -582,7 +582,7 @@
         <v>5350</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>30.9</v>
@@ -638,7 +638,7 @@
         <v>715</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>90.38</v>
@@ -694,7 +694,7 @@
         <v>1367</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>125.35</v>
@@ -761,13 +761,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -775,13 +775,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>5350</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -792,13 +792,13 @@
         <v>502</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>5350</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -809,27 +809,27 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -840,13 +840,13 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>502</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>0.49748999999999999</v>

</xml_diff>